<commit_message>
Done, it's working #177
</commit_message>
<xml_diff>
--- a/Lists/ideac.xlsx
+++ b/Lists/ideac.xlsx
@@ -1206,8 +1206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59:XFD59"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2207,7 +2207,7 @@
         <v>82</v>
       </c>
       <c r="C42" s="2">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>0</v>
@@ -2633,5 +2633,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>